<commit_message>
with GS Update check - 11/04/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 3.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 3.3 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3936092E-78A5-4AC0-B66F-FE351AACFB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C70D6C3-B5F1-44EA-9459-56BD526AB734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5127" uniqueCount="1281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5129" uniqueCount="1281">
   <si>
     <t>PS</t>
   </si>
@@ -4547,10 +4547,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1858"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="N1828" sqref="N1828"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -24066,7 +24066,9 @@
       <c r="V500" s="44"/>
     </row>
     <row r="501" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A501" s="7"/>
+      <c r="A501" s="7" t="s">
+        <v>112</v>
+      </c>
       <c r="D501" s="25"/>
       <c r="E501" s="20"/>
       <c r="F501" s="20"/>
@@ -64930,7 +64932,7 @@
       </c>
       <c r="V1712" s="44"/>
     </row>
-    <row r="1713" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1713" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1713" s="51" t="s">
         <v>104</v>
       </c>
@@ -64957,7 +64959,7 @@
       </c>
       <c r="V1713" s="44"/>
     </row>
-    <row r="1714" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1714" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1714" s="51" t="s">
         <v>104</v>
       </c>
@@ -64984,7 +64986,7 @@
       </c>
       <c r="V1714" s="44"/>
     </row>
-    <row r="1715" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1715" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1715" s="51" t="s">
         <v>104</v>
       </c>
@@ -65011,7 +65013,7 @@
       </c>
       <c r="V1715" s="44"/>
     </row>
-    <row r="1716" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1716" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1716" s="51" t="s">
         <v>104</v>
       </c>
@@ -65041,7 +65043,7 @@
       </c>
       <c r="V1716" s="44"/>
     </row>
-    <row r="1717" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1717" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1717" s="51" t="s">
         <v>104</v>
       </c>
@@ -65076,7 +65078,10 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="1718" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1718" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A1718" s="53" t="s">
+        <v>123</v>
+      </c>
       <c r="C1718" s="51" t="s">
         <v>104</v>
       </c>
@@ -65112,7 +65117,7 @@
       </c>
       <c r="V1718" s="44"/>
     </row>
-    <row r="1719" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1719" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1719" s="51" t="s">
         <v>104</v>
       </c>
@@ -65142,7 +65147,7 @@
       </c>
       <c r="V1719" s="44"/>
     </row>
-    <row r="1720" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1720" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1720" s="51" t="s">
         <v>104</v>
       </c>
@@ -65172,7 +65177,7 @@
       </c>
       <c r="V1720" s="44"/>
     </row>
-    <row r="1721" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1721" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1721" s="51" t="s">
         <v>104</v>
       </c>
@@ -65207,7 +65212,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="1722" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1722" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1722" s="51" t="s">
         <v>104</v>
       </c>
@@ -65237,7 +65242,7 @@
       </c>
       <c r="V1722" s="44"/>
     </row>
-    <row r="1723" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1723" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1723" s="51" t="s">
         <v>104</v>
       </c>
@@ -65264,7 +65269,7 @@
       </c>
       <c r="V1723" s="44"/>
     </row>
-    <row r="1724" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1724" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1724" s="51" t="s">
         <v>104</v>
       </c>
@@ -65296,7 +65301,7 @@
         <v>1261</v>
       </c>
     </row>
-    <row r="1725" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1725" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1725" s="51" t="s">
         <v>104</v>
       </c>
@@ -65323,7 +65328,7 @@
       </c>
       <c r="V1725" s="44"/>
     </row>
-    <row r="1726" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1726" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1726" s="51" t="s">
         <v>104</v>
       </c>
@@ -65350,7 +65355,7 @@
       </c>
       <c r="V1726" s="44"/>
     </row>
-    <row r="1727" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1727" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1727" s="51" t="s">
         <v>104</v>
       </c>
@@ -65382,7 +65387,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="1728" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1728" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1728" s="51" t="s">
         <v>104</v>
       </c>

</xml_diff>

<commit_message>
Padam Templates edits - 25/04/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 3.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 3.3 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C70D6C3-B5F1-44EA-9459-56BD526AB734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF742B3D-C99B-4F2B-9412-AE24D5398EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5129" uniqueCount="1281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5132" uniqueCount="1281">
   <si>
     <t>PS</t>
   </si>
@@ -4033,12 +4033,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -4046,6 +4040,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4077,7 +4077,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4244,9 +4244,6 @@
     <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4263,6 +4260,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -4547,10 +4550,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1858"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A192" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N1828" sqref="N1828"/>
+      <selection pane="bottomLeft" activeCell="O201" sqref="O201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -9809,7 +9812,7 @@
         <f t="shared" si="5"/>
         <v>123</v>
       </c>
-      <c r="N124" s="57" t="s">
+      <c r="N124" s="55" t="s">
         <v>182</v>
       </c>
       <c r="O124" s="6"/>
@@ -12697,7 +12700,7 @@
         <f t="shared" si="11"/>
         <v>76</v>
       </c>
-      <c r="N200" s="58" t="s">
+      <c r="N200" s="57" t="s">
         <v>240</v>
       </c>
       <c r="O200" s="6"/>
@@ -12736,7 +12739,7 @@
         <f t="shared" si="11"/>
         <v>77</v>
       </c>
-      <c r="N201" s="58" t="s">
+      <c r="N201" s="57" t="s">
         <v>241</v>
       </c>
       <c r="O201" s="6" t="s">
@@ -12777,7 +12780,7 @@
         <f t="shared" si="11"/>
         <v>78</v>
       </c>
-      <c r="N202" s="57" t="s">
+      <c r="N202" s="55" t="s">
         <v>1139</v>
       </c>
       <c r="O202" s="6"/>
@@ -19437,7 +19440,7 @@
         <f t="shared" si="17"/>
         <v>175</v>
       </c>
-      <c r="N377" s="57" t="s">
+      <c r="N377" s="56" t="s">
         <v>744</v>
       </c>
       <c r="O377" s="6"/>
@@ -20468,7 +20471,7 @@
     </row>
     <row r="405" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A405" s="7"/>
-      <c r="D405" s="59"/>
+      <c r="D405" s="58"/>
       <c r="E405" s="20"/>
       <c r="F405" s="20"/>
       <c r="G405" s="20"/>
@@ -22516,7 +22519,7 @@
       <c r="A460" s="7"/>
       <c r="B460" s="39"/>
       <c r="D460" s="25"/>
-      <c r="E460" s="60"/>
+      <c r="E460" s="59"/>
       <c r="F460" s="20"/>
       <c r="G460" s="20"/>
       <c r="H460" s="20"/>
@@ -22553,7 +22556,7 @@
     <row r="461" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A461" s="7"/>
       <c r="D461" s="25"/>
-      <c r="E461" s="60"/>
+      <c r="E461" s="59"/>
       <c r="F461" s="20"/>
       <c r="G461" s="20"/>
       <c r="H461" s="20"/>
@@ -24013,7 +24016,9 @@
       <c r="N499" s="44" t="s">
         <v>367</v>
       </c>
-      <c r="O499" s="7"/>
+      <c r="O499" s="64" t="s">
+        <v>1</v>
+      </c>
       <c r="P499" s="7"/>
       <c r="Q499" s="7"/>
       <c r="R499" s="7"/>
@@ -25193,7 +25198,7 @@
         <f t="shared" si="26"/>
         <v>153</v>
       </c>
-      <c r="N530" s="57" t="s">
+      <c r="N530" s="56" t="s">
         <v>1143</v>
       </c>
       <c r="O530" s="6"/>
@@ -25442,7 +25447,7 @@
         <v>125</v>
       </c>
       <c r="D537" s="25"/>
-      <c r="E537" s="61" t="s">
+      <c r="E537" s="60" t="s">
         <v>124</v>
       </c>
       <c r="F537" s="20"/>
@@ -25487,7 +25492,7 @@
         <v>125</v>
       </c>
       <c r="D538" s="25"/>
-      <c r="E538" s="61" t="s">
+      <c r="E538" s="60" t="s">
         <v>124</v>
       </c>
       <c r="F538" s="20"/>
@@ -33956,7 +33961,7 @@
         <f t="shared" si="38"/>
         <v>246</v>
       </c>
-      <c r="N776" s="57" t="s">
+      <c r="N776" s="55" t="s">
         <v>379</v>
       </c>
       <c r="O776" s="6"/>
@@ -37416,7 +37421,9 @@
       <c r="N881" s="44" t="s">
         <v>241</v>
       </c>
-      <c r="O881" s="6"/>
+      <c r="O881" s="65" t="s">
+        <v>1</v>
+      </c>
       <c r="P881" s="7"/>
       <c r="Q881" s="7"/>
       <c r="R881" s="7"/>
@@ -38782,7 +38789,9 @@
       <c r="N922" s="44" t="s">
         <v>241</v>
       </c>
-      <c r="O922" s="6"/>
+      <c r="O922" s="65" t="s">
+        <v>1</v>
+      </c>
       <c r="P922" s="7"/>
       <c r="Q922" s="7"/>
       <c r="R922" s="7"/>
@@ -38854,7 +38863,7 @@
         <f t="shared" si="44"/>
         <v>148</v>
       </c>
-      <c r="N924" s="57" t="s">
+      <c r="N924" s="56" t="s">
         <v>511</v>
       </c>
       <c r="O924" s="32"/>
@@ -39027,7 +39036,7 @@
         <f t="shared" si="44"/>
         <v>5</v>
       </c>
-      <c r="N929" s="58" t="s">
+      <c r="N929" s="57" t="s">
         <v>241</v>
       </c>
       <c r="O929" s="6" t="s">
@@ -39064,7 +39073,7 @@
         <f t="shared" si="44"/>
         <v>6</v>
       </c>
-      <c r="N930" s="58" t="s">
+      <c r="N930" s="57" t="s">
         <v>518</v>
       </c>
       <c r="O930" s="6"/>
@@ -39389,7 +39398,7 @@
         <f t="shared" si="44"/>
         <v>16</v>
       </c>
-      <c r="N940" s="58" t="s">
+      <c r="N940" s="57" t="s">
         <v>241</v>
       </c>
       <c r="O940" s="6" t="s">
@@ -39426,7 +39435,7 @@
         <f t="shared" si="44"/>
         <v>17</v>
       </c>
-      <c r="N941" s="58" t="s">
+      <c r="N941" s="57" t="s">
         <v>518</v>
       </c>
       <c r="O941" s="6"/>
@@ -44074,7 +44083,7 @@
         <f t="shared" si="50"/>
         <v>158</v>
       </c>
-      <c r="N1082" s="57" t="s">
+      <c r="N1082" s="55" t="s">
         <v>1144</v>
       </c>
       <c r="O1082" s="6"/>
@@ -47873,16 +47882,16 @@
       <c r="V1192" s="44"/>
     </row>
     <row r="1193" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="D1193" s="62" t="s">
+      <c r="D1193" s="61" t="s">
         <v>126</v>
       </c>
-      <c r="E1193" s="61" t="s">
+      <c r="E1193" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="F1193" s="61" t="s">
+      <c r="F1193" s="60" t="s">
         <v>128</v>
       </c>
-      <c r="G1193" s="61" t="s">
+      <c r="G1193" s="60" t="s">
         <v>131</v>
       </c>
       <c r="H1193" s="50" t="s">
@@ -47916,16 +47925,16 @@
       <c r="V1193" s="44"/>
     </row>
     <row r="1194" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="D1194" s="62" t="s">
+      <c r="D1194" s="61" t="s">
         <v>126</v>
       </c>
-      <c r="E1194" s="61" t="s">
+      <c r="E1194" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="F1194" s="61" t="s">
+      <c r="F1194" s="60" t="s">
         <v>128</v>
       </c>
-      <c r="G1194" s="61" t="s">
+      <c r="G1194" s="60" t="s">
         <v>131</v>
       </c>
       <c r="H1194" s="50" t="s">
@@ -54311,7 +54320,7 @@
         <f t="shared" si="65"/>
         <v>300</v>
       </c>
-      <c r="N1382" s="57" t="s">
+      <c r="N1382" s="55" t="s">
         <v>1153</v>
       </c>
       <c r="O1382" s="32"/>
@@ -55138,10 +55147,10 @@
     </row>
     <row r="1407" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1407" s="42"/>
-      <c r="D1407" s="62" t="s">
+      <c r="D1407" s="61" t="s">
         <v>129</v>
       </c>
-      <c r="E1407" s="61" t="s">
+      <c r="E1407" s="60" t="s">
         <v>130</v>
       </c>
       <c r="F1407" s="20"/>
@@ -55167,7 +55176,7 @@
         <f t="shared" si="65"/>
         <v>25</v>
       </c>
-      <c r="N1407" s="56" t="s">
+      <c r="N1407" s="55" t="s">
         <v>729</v>
       </c>
       <c r="O1407" s="6"/>
@@ -55178,10 +55187,10 @@
     </row>
     <row r="1408" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1408" s="42"/>
-      <c r="D1408" s="62" t="s">
+      <c r="D1408" s="61" t="s">
         <v>129</v>
       </c>
-      <c r="E1408" s="61" t="s">
+      <c r="E1408" s="60" t="s">
         <v>130</v>
       </c>
       <c r="F1408" s="20"/>
@@ -55207,7 +55216,7 @@
         <f t="shared" si="65"/>
         <v>26</v>
       </c>
-      <c r="N1408" s="56" t="s">
+      <c r="N1408" s="55" t="s">
         <v>730</v>
       </c>
       <c r="O1408" s="6"/>
@@ -58036,7 +58045,7 @@
         <f t="shared" si="71"/>
         <v>108</v>
       </c>
-      <c r="N1490" s="57" t="s">
+      <c r="N1490" s="56" t="s">
         <v>770</v>
       </c>
       <c r="O1490" s="7"/>
@@ -61208,7 +61217,7 @@
         <f t="shared" si="74"/>
         <v>94</v>
       </c>
-      <c r="N1584" s="57" t="s">
+      <c r="N1584" s="56" t="s">
         <v>1168</v>
       </c>
       <c r="O1584" s="7" t="s">
@@ -68329,10 +68338,10 @@
       <c r="C1827" s="51" t="s">
         <v>104</v>
       </c>
-      <c r="D1827" s="62" t="s">
+      <c r="D1827" s="61" t="s">
         <v>132</v>
       </c>
-      <c r="G1827" s="63" t="s">
+      <c r="G1827" s="62" t="s">
         <v>133</v>
       </c>
       <c r="H1827" s="50" t="s">
@@ -68368,10 +68377,10 @@
       <c r="C1828" s="51" t="s">
         <v>104</v>
       </c>
-      <c r="D1828" s="62" t="s">
+      <c r="D1828" s="61" t="s">
         <v>132</v>
       </c>
-      <c r="G1828" s="63" t="s">
+      <c r="G1828" s="62" t="s">
         <v>133</v>
       </c>
       <c r="H1828" s="50" t="s">
@@ -69240,10 +69249,10 @@
         <f t="shared" si="86"/>
         <v>274</v>
       </c>
-      <c r="N1858" s="57" t="s">
+      <c r="N1858" s="56" t="s">
         <v>182</v>
       </c>
-      <c r="O1858" s="64"/>
+      <c r="O1858" s="63"/>
       <c r="P1858" s="7" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
TS Padam Excel corrections - 30/08/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 3.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 3.3 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF742B3D-C99B-4F2B-9412-AE24D5398EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836D2F1B-84AE-4946-AE87-0B7E5F12104F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4018,7 +4018,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4028,12 +4028,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4077,7 +4071,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4241,9 +4235,6 @@
     <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4262,10 +4253,10 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -4550,10 +4541,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1858"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A192" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="O201" sqref="O201"/>
+      <selection pane="bottomLeft" activeCell="N1858" sqref="N1858"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -12700,7 +12691,7 @@
         <f t="shared" si="11"/>
         <v>76</v>
       </c>
-      <c r="N200" s="57" t="s">
+      <c r="N200" s="56" t="s">
         <v>240</v>
       </c>
       <c r="O200" s="6"/>
@@ -12739,7 +12730,7 @@
         <f t="shared" si="11"/>
         <v>77</v>
       </c>
-      <c r="N201" s="57" t="s">
+      <c r="N201" s="56" t="s">
         <v>241</v>
       </c>
       <c r="O201" s="6" t="s">
@@ -19440,7 +19431,7 @@
         <f t="shared" si="17"/>
         <v>175</v>
       </c>
-      <c r="N377" s="56" t="s">
+      <c r="N377" s="55" t="s">
         <v>744</v>
       </c>
       <c r="O377" s="6"/>
@@ -20471,7 +20462,7 @@
     </row>
     <row r="405" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A405" s="7"/>
-      <c r="D405" s="58"/>
+      <c r="D405" s="57"/>
       <c r="E405" s="20"/>
       <c r="F405" s="20"/>
       <c r="G405" s="20"/>
@@ -22519,7 +22510,7 @@
       <c r="A460" s="7"/>
       <c r="B460" s="39"/>
       <c r="D460" s="25"/>
-      <c r="E460" s="59"/>
+      <c r="E460" s="58"/>
       <c r="F460" s="20"/>
       <c r="G460" s="20"/>
       <c r="H460" s="20"/>
@@ -22556,7 +22547,7 @@
     <row r="461" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A461" s="7"/>
       <c r="D461" s="25"/>
-      <c r="E461" s="59"/>
+      <c r="E461" s="58"/>
       <c r="F461" s="20"/>
       <c r="G461" s="20"/>
       <c r="H461" s="20"/>
@@ -24016,7 +24007,7 @@
       <c r="N499" s="44" t="s">
         <v>367</v>
       </c>
-      <c r="O499" s="64" t="s">
+      <c r="O499" s="63" t="s">
         <v>1</v>
       </c>
       <c r="P499" s="7"/>
@@ -25198,7 +25189,7 @@
         <f t="shared" si="26"/>
         <v>153</v>
       </c>
-      <c r="N530" s="56" t="s">
+      <c r="N530" s="55" t="s">
         <v>1143</v>
       </c>
       <c r="O530" s="6"/>
@@ -25447,7 +25438,7 @@
         <v>125</v>
       </c>
       <c r="D537" s="25"/>
-      <c r="E537" s="60" t="s">
+      <c r="E537" s="59" t="s">
         <v>124</v>
       </c>
       <c r="F537" s="20"/>
@@ -25492,7 +25483,7 @@
         <v>125</v>
       </c>
       <c r="D538" s="25"/>
-      <c r="E538" s="60" t="s">
+      <c r="E538" s="59" t="s">
         <v>124</v>
       </c>
       <c r="F538" s="20"/>
@@ -37421,7 +37412,7 @@
       <c r="N881" s="44" t="s">
         <v>241</v>
       </c>
-      <c r="O881" s="65" t="s">
+      <c r="O881" s="64" t="s">
         <v>1</v>
       </c>
       <c r="P881" s="7"/>
@@ -38789,7 +38780,7 @@
       <c r="N922" s="44" t="s">
         <v>241</v>
       </c>
-      <c r="O922" s="65" t="s">
+      <c r="O922" s="64" t="s">
         <v>1</v>
       </c>
       <c r="P922" s="7"/>
@@ -38863,7 +38854,7 @@
         <f t="shared" si="44"/>
         <v>148</v>
       </c>
-      <c r="N924" s="56" t="s">
+      <c r="N924" s="55" t="s">
         <v>511</v>
       </c>
       <c r="O924" s="32"/>
@@ -39036,7 +39027,7 @@
         <f t="shared" si="44"/>
         <v>5</v>
       </c>
-      <c r="N929" s="57" t="s">
+      <c r="N929" s="56" t="s">
         <v>241</v>
       </c>
       <c r="O929" s="6" t="s">
@@ -39073,7 +39064,7 @@
         <f t="shared" si="44"/>
         <v>6</v>
       </c>
-      <c r="N930" s="57" t="s">
+      <c r="N930" s="56" t="s">
         <v>518</v>
       </c>
       <c r="O930" s="6"/>
@@ -39398,7 +39389,7 @@
         <f t="shared" si="44"/>
         <v>16</v>
       </c>
-      <c r="N940" s="57" t="s">
+      <c r="N940" s="56" t="s">
         <v>241</v>
       </c>
       <c r="O940" s="6" t="s">
@@ -39435,7 +39426,7 @@
         <f t="shared" si="44"/>
         <v>17</v>
       </c>
-      <c r="N941" s="57" t="s">
+      <c r="N941" s="56" t="s">
         <v>518</v>
       </c>
       <c r="O941" s="6"/>
@@ -47882,16 +47873,16 @@
       <c r="V1192" s="44"/>
     </row>
     <row r="1193" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="D1193" s="61" t="s">
+      <c r="D1193" s="60" t="s">
         <v>126</v>
       </c>
-      <c r="E1193" s="60" t="s">
+      <c r="E1193" s="59" t="s">
         <v>127</v>
       </c>
-      <c r="F1193" s="60" t="s">
+      <c r="F1193" s="59" t="s">
         <v>128</v>
       </c>
-      <c r="G1193" s="60" t="s">
+      <c r="G1193" s="59" t="s">
         <v>131</v>
       </c>
       <c r="H1193" s="50" t="s">
@@ -47925,16 +47916,16 @@
       <c r="V1193" s="44"/>
     </row>
     <row r="1194" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="D1194" s="61" t="s">
+      <c r="D1194" s="60" t="s">
         <v>126</v>
       </c>
-      <c r="E1194" s="60" t="s">
+      <c r="E1194" s="59" t="s">
         <v>127</v>
       </c>
-      <c r="F1194" s="60" t="s">
+      <c r="F1194" s="59" t="s">
         <v>128</v>
       </c>
-      <c r="G1194" s="60" t="s">
+      <c r="G1194" s="59" t="s">
         <v>131</v>
       </c>
       <c r="H1194" s="50" t="s">
@@ -55147,10 +55138,10 @@
     </row>
     <row r="1407" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1407" s="42"/>
-      <c r="D1407" s="61" t="s">
+      <c r="D1407" s="60" t="s">
         <v>129</v>
       </c>
-      <c r="E1407" s="60" t="s">
+      <c r="E1407" s="59" t="s">
         <v>130</v>
       </c>
       <c r="F1407" s="20"/>
@@ -55187,10 +55178,10 @@
     </row>
     <row r="1408" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="C1408" s="42"/>
-      <c r="D1408" s="61" t="s">
+      <c r="D1408" s="60" t="s">
         <v>129</v>
       </c>
-      <c r="E1408" s="60" t="s">
+      <c r="E1408" s="59" t="s">
         <v>130</v>
       </c>
       <c r="F1408" s="20"/>
@@ -58045,7 +58036,7 @@
         <f t="shared" si="71"/>
         <v>108</v>
       </c>
-      <c r="N1490" s="56" t="s">
+      <c r="N1490" s="55" t="s">
         <v>770</v>
       </c>
       <c r="O1490" s="7"/>
@@ -61217,7 +61208,7 @@
         <f t="shared" si="74"/>
         <v>94</v>
       </c>
-      <c r="N1584" s="56" t="s">
+      <c r="N1584" s="55" t="s">
         <v>1168</v>
       </c>
       <c r="O1584" s="7" t="s">
@@ -68338,10 +68329,10 @@
       <c r="C1827" s="51" t="s">
         <v>104</v>
       </c>
-      <c r="D1827" s="61" t="s">
+      <c r="D1827" s="60" t="s">
         <v>132</v>
       </c>
-      <c r="G1827" s="62" t="s">
+      <c r="G1827" s="61" t="s">
         <v>133</v>
       </c>
       <c r="H1827" s="50" t="s">
@@ -68377,10 +68368,10 @@
       <c r="C1828" s="51" t="s">
         <v>104</v>
       </c>
-      <c r="D1828" s="61" t="s">
+      <c r="D1828" s="60" t="s">
         <v>132</v>
       </c>
-      <c r="G1828" s="62" t="s">
+      <c r="G1828" s="61" t="s">
         <v>133</v>
       </c>
       <c r="H1828" s="50" t="s">
@@ -69249,10 +69240,10 @@
         <f t="shared" si="86"/>
         <v>274</v>
       </c>
-      <c r="N1858" s="56" t="s">
+      <c r="N1858" s="55" t="s">
         <v>182</v>
       </c>
-      <c r="O1858" s="63"/>
+      <c r="O1858" s="62"/>
       <c r="P1858" s="7" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
TS 3.3 and 6.2 Padam Templates - 25/09/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 3.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 3.3 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62ED9EB-FBDE-4352-AEE3-C1C4AFA80E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6D0570-132D-44BF-9859-EA65C5CFD757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4513,10 +4513,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1858"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V2" sqref="V2"/>
+      <selection pane="bottomLeft" activeCell="N422" sqref="N422"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
nmv 29 09 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 3.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 3.3 Padam Input Template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6D0570-132D-44BF-9859-EA65C5CFD757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="TS 3.3" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TS 3.3'!$C$1:$V$1858</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6671" uniqueCount="1282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6672" uniqueCount="1282">
   <si>
     <t>PS</t>
   </si>
@@ -3887,8 +3886,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4020,6 +4019,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -4074,7 +4080,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4230,6 +4236,9 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4510,13 +4519,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V1858"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1845" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N422" sqref="N422"/>
+      <selection pane="bottomLeft" activeCell="N1862" sqref="N1862"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -17540,7 +17549,9 @@
       <c r="N338" s="37" t="s">
         <v>328</v>
       </c>
-      <c r="O338" s="6"/>
+      <c r="O338" s="53" t="s">
+        <v>1</v>
+      </c>
       <c r="P338" s="7" t="s">
         <v>19</v>
       </c>
@@ -44299,7 +44310,7 @@
       <c r="P1147" s="7"/>
       <c r="Q1147" s="7"/>
       <c r="R1147" s="7"/>
-      <c r="U1147" s="7" t="s">
+      <c r="U1147" s="54" t="s">
         <v>82</v>
       </c>
       <c r="V1147" s="37" t="s">

</xml_diff>

<commit_message>
nmv 08 10 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 3.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 3.3 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4B1D3D-66D2-4428-8027-1B6D3C4E4156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6DE30D-8416-44AB-B1E3-158406EAB20D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="472" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6672" uniqueCount="1281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6673" uniqueCount="1282">
   <si>
     <t>PS</t>
   </si>
@@ -3882,6 +3882,9 @@
   </si>
   <si>
     <t>suqpAqNiH</t>
+  </si>
+  <si>
+    <t>yaqj~jo &amp;nu, yaqj~jo anvanu</t>
   </si>
 </sst>
 </file>
@@ -4021,7 +4024,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4049,6 +4052,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4080,7 +4089,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4245,6 +4254,12 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4526,12 +4541,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V1858"/>
+  <dimension ref="A1:AA1858"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1815" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A923" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N1822" sqref="N1822"/>
+      <selection pane="bottomLeft" activeCell="V933" sqref="V933"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -4555,7 +4570,8 @@
     <col min="20" max="20" width="23.140625" style="7" customWidth="1"/>
     <col min="21" max="21" width="18.5703125" style="7" customWidth="1"/>
     <col min="22" max="22" width="62.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="262" width="9.140625" style="2"/>
+    <col min="23" max="23" width="39.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="262" width="9.140625" style="2"/>
     <col min="263" max="263" width="9.28515625" style="2" customWidth="1"/>
     <col min="264" max="265" width="9.140625" style="2"/>
     <col min="266" max="266" width="54.42578125" style="2" customWidth="1"/>
@@ -37376,7 +37392,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="929" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="929" spans="1:27" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I929" s="36" t="s">
         <v>42</v>
       </c>
@@ -37410,8 +37426,15 @@
       <c r="V929" s="37" t="s">
         <v>1274</v>
       </c>
-    </row>
-    <row r="930" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="W929" s="57" t="s">
+        <v>1281</v>
+      </c>
+      <c r="X929" s="58"/>
+      <c r="Y929" s="58"/>
+      <c r="Z929" s="58"/>
+      <c r="AA929" s="58"/>
+    </row>
+    <row r="930" spans="1:27" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I930" s="36" t="s">
         <v>42</v>
       </c>
@@ -37441,7 +37464,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="931" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="931" spans="1:27" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I931" s="36" t="s">
         <v>42</v>
       </c>
@@ -37471,7 +37494,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="932" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="932" spans="1:27" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I932" s="36" t="s">
         <v>42</v>
       </c>
@@ -37501,7 +37524,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="933" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="933" spans="1:27" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I933" s="36" t="s">
         <v>42</v>
       </c>
@@ -37531,7 +37554,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="934" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="934" spans="1:27" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I934" s="36" t="s">
         <v>42</v>
       </c>
@@ -37561,7 +37584,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="935" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="935" spans="1:27" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I935" s="36" t="s">
         <v>42</v>
       </c>
@@ -37591,7 +37614,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="936" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="936" spans="1:27" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I936" s="36" t="s">
         <v>42</v>
       </c>
@@ -37623,7 +37646,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="937" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="937" spans="1:27" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I937" s="36" t="s">
         <v>42</v>
       </c>
@@ -37653,7 +37676,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="938" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="938" spans="1:27" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I938" s="36" t="s">
         <v>42</v>
       </c>
@@ -37683,7 +37706,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="939" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="939" spans="1:27" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I939" s="36" t="s">
         <v>42</v>
       </c>
@@ -37713,7 +37736,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="940" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="940" spans="1:27" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A940" s="46" t="s">
         <v>119</v>
       </c>
@@ -37751,7 +37774,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="941" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="941" spans="1:27" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I941" s="36" t="s">
         <v>42</v>
       </c>
@@ -37781,7 +37804,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="942" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="942" spans="1:27" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I942" s="36" t="s">
         <v>42</v>
       </c>
@@ -37813,7 +37836,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="943" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="943" spans="1:27" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I943" s="36" t="s">
         <v>42</v>
       </c>
@@ -37843,7 +37866,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="944" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="944" spans="1:27" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I944" s="36" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
nmv 10 10 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 3.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 3.3 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244D4698-32C0-430B-B1D2-B608091DEDC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56A352B-528F-4476-B169-459D34EE8CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="472" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TS 3.3'!$A$1:$XER$1858</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,12 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6673" uniqueCount="1282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6675" uniqueCount="1283">
   <si>
     <t>PS</t>
   </si>
@@ -3919,6 +3916,9 @@
       </rPr>
       <t>qkAqShTaqkAyA$m</t>
     </r>
+  </si>
+  <si>
+    <t>Sh</t>
   </si>
 </sst>
 </file>
@@ -4129,7 +4129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4299,6 +4299,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4583,10 +4595,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1858"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1262" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1586" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N1273" sqref="N1273"/>
+      <selection pane="bottomLeft" activeCell="N1598" sqref="N1598"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -58777,12 +58789,18 @@
         <f t="shared" si="74"/>
         <v>13</v>
       </c>
-      <c r="N1597" s="37" t="s">
+      <c r="N1597" s="59" t="s">
         <v>326</v>
       </c>
-      <c r="O1597" s="6" t="s">
+      <c r="O1597" s="60" t="s">
         <v>1</v>
       </c>
+      <c r="P1597" s="61"/>
+      <c r="Q1597" s="61"/>
+      <c r="R1597" s="61"/>
+      <c r="S1597" s="62"/>
+      <c r="T1597" s="62"/>
+      <c r="U1597" s="62"/>
       <c r="V1597" s="37" t="s">
         <v>1272</v>
       </c>
@@ -58811,6 +58829,12 @@
       </c>
       <c r="N1598" s="37" t="s">
         <v>815</v>
+      </c>
+      <c r="S1598" s="52" t="s">
+        <v>107</v>
+      </c>
+      <c r="T1598" s="52" t="s">
+        <v>1282</v>
       </c>
       <c r="V1598" s="37" t="s">
         <v>1272</v>

</xml_diff>

<commit_message>
nmv 12 10 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 3.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 3.3 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56A352B-528F-4476-B169-459D34EE8CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4BEC42-026B-4463-B378-53AE248A7702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="472" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4129,7 +4129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4299,18 +4299,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4598,7 +4586,7 @@
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1586" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N1598" sqref="N1598"/>
+      <selection pane="bottomLeft" activeCell="S1598" sqref="S1598"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -58789,18 +58777,12 @@
         <f t="shared" si="74"/>
         <v>13</v>
       </c>
-      <c r="N1597" s="59" t="s">
+      <c r="N1597" s="37" t="s">
         <v>326</v>
       </c>
-      <c r="O1597" s="60" t="s">
+      <c r="O1597" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="P1597" s="61"/>
-      <c r="Q1597" s="61"/>
-      <c r="R1597" s="61"/>
-      <c r="S1597" s="62"/>
-      <c r="T1597" s="62"/>
-      <c r="U1597" s="62"/>
       <c r="V1597" s="37" t="s">
         <v>1272</v>
       </c>
@@ -58831,10 +58813,10 @@
         <v>815</v>
       </c>
       <c r="S1598" s="52" t="s">
+        <v>1282</v>
+      </c>
+      <c r="T1598" s="52" t="s">
         <v>107</v>
-      </c>
-      <c r="T1598" s="52" t="s">
-        <v>1282</v>
       </c>
       <c r="V1598" s="37" t="s">
         <v>1272</v>

</xml_diff>

<commit_message>
nmv 07 11 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 3.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 3.3 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEF90E3-DF05-43B5-A6B0-37DF9D486CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C68893-0359-4B78-9D44-106E15F1321A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="472" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6682" uniqueCount="1283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6673" uniqueCount="1283">
   <si>
     <t>PS</t>
   </si>
@@ -4575,10 +4575,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1858"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1484" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A976" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N1493" sqref="N1493"/>
+      <selection pane="bottomLeft" activeCell="U940" sqref="U940"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -37452,9 +37452,6 @@
       <c r="P929" s="7"/>
       <c r="Q929" s="7"/>
       <c r="R929" s="7"/>
-      <c r="U929" s="7" t="s">
-        <v>88</v>
-      </c>
       <c r="V929" s="37" t="s">
         <v>1262</v>
       </c>
@@ -37799,9 +37796,6 @@
       <c r="P940" s="7"/>
       <c r="Q940" s="7"/>
       <c r="R940" s="7"/>
-      <c r="U940" s="7" t="s">
-        <v>88</v>
-      </c>
       <c r="V940" s="37" t="s">
         <v>1262</v>
       </c>

</xml_diff>

<commit_message>
nmv 21 11 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 3.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 3.3 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD56DFD-1E72-4943-B132-F5930BDFA007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4413C561-AAD0-4B03-BD85-F82231EB6062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="472" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6673" uniqueCount="1283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6672" uniqueCount="1282">
   <si>
     <t>PS</t>
   </si>
@@ -3829,9 +3829,6 @@
   </si>
   <si>
     <t>suqpAqNiH</t>
-  </si>
-  <si>
-    <t>yaqj~jo &amp;nu, yaqj~jo anvanu</t>
   </si>
   <si>
     <r>
@@ -4056,7 +4053,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4084,12 +4081,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4287,10 +4278,10 @@
     <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4576,9 +4567,9 @@
   <dimension ref="A1:AA1858"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1678" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A925" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="M1688" sqref="M1688"/>
+      <selection pane="bottomLeft" activeCell="N930" sqref="N930"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -32461,7 +32452,7 @@
         <v>238</v>
       </c>
       <c r="N768" s="38" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="O768" s="7" t="s">
         <v>0</v>
@@ -34270,7 +34261,7 @@
         <v>51</v>
       </c>
       <c r="N827" s="38" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="O827" s="7" t="s">
         <v>0</v>
@@ -35041,7 +35032,7 @@
         <v>76</v>
       </c>
       <c r="N852" s="38" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="O852" s="7" t="s">
         <v>0</v>
@@ -37455,9 +37446,7 @@
       <c r="V929" s="37" t="s">
         <v>1260</v>
       </c>
-      <c r="W929" s="57" t="s">
-        <v>1267</v>
-      </c>
+      <c r="W929" s="57"/>
       <c r="X929" s="58"/>
       <c r="Y929" s="58"/>
       <c r="Z929" s="58"/>
@@ -43567,7 +43556,7 @@
         <v>40</v>
       </c>
       <c r="N1122" s="38" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="O1122" s="7" t="s">
         <v>0</v>
@@ -48373,7 +48362,7 @@
         <v>191</v>
       </c>
       <c r="N1273" s="56" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="O1273" s="7" t="s">
         <v>0</v>
@@ -48382,7 +48371,7 @@
       <c r="Q1273" s="7"/>
       <c r="R1273" s="7"/>
       <c r="V1273" s="56" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="1274" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55485,7 +55474,7 @@
         <v>3</v>
       </c>
       <c r="N1493" s="38" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O1493" s="7" t="s">
         <v>0</v>
@@ -57686,7 +57675,7 @@
         <v>72</v>
       </c>
       <c r="N1562" s="38" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="O1562" s="7" t="s">
         <v>0</v>
@@ -57782,7 +57771,7 @@
         <v>75</v>
       </c>
       <c r="N1565" s="38" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="O1565" s="7" t="s">
         <v>0</v>
@@ -57814,7 +57803,7 @@
         <v>76</v>
       </c>
       <c r="N1566" s="38" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="O1566" s="7" t="s">
         <v>0</v>
@@ -57846,7 +57835,7 @@
         <v>77</v>
       </c>
       <c r="N1567" s="38" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="O1567" s="7" t="s">
         <v>0</v>
@@ -58551,7 +58540,7 @@
         <v>6</v>
       </c>
       <c r="N1590" s="38" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="O1590" s="7" t="s">
         <v>17</v>
@@ -58798,7 +58787,7 @@
         <v>807</v>
       </c>
       <c r="S1598" s="52" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="T1598" s="52" t="s">
         <v>107</v>
@@ -58859,7 +58848,7 @@
         <v>16</v>
       </c>
       <c r="N1600" s="38" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="O1600" s="7" t="s">
         <v>17</v>
@@ -59016,7 +59005,7 @@
         <v>21</v>
       </c>
       <c r="N1605" s="38" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="O1605" s="7" t="s">
         <v>17</v>
@@ -60549,7 +60538,7 @@
         <v>71</v>
       </c>
       <c r="N1655" s="38" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="O1655" s="7" t="s">
         <v>0</v>
@@ -61081,7 +61070,7 @@
         <v>0</v>
       </c>
       <c r="V1672" s="38" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="1673" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61544,7 +61533,7 @@
         <v>104</v>
       </c>
       <c r="N1688" s="38" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="O1688" s="7" t="s">
         <v>0</v>

</xml_diff>